<commit_message>
Review comment changes done for fireclass Hungary and UK zettler for UK
</commit_message>
<xml_diff>
--- a/Test Data/AttachedFunctionality_PFI_Node_XX_Panel.xlsx
+++ b/Test Data/AttachedFunctionality_PFI_Node_XX_Panel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8683FA-3628-4683-81FF-EA8935CB35BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E80F6AC-73ED-4225-9C27-EBA2CDAE3ACC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="19" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
@@ -228,10 +228,10 @@
     <t>Poland Market</t>
   </si>
   <si>
-    <t>NGC-2741/T3343</t>
-  </si>
-  <si>
     <t>UK Market</t>
+  </si>
+  <si>
+    <t>NGC-2741/T3344</t>
   </si>
 </sst>
 </file>
@@ -1988,7 +1988,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2011,7 +2011,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -2033,7 +2033,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">

</xml_diff>